<commit_message>
preparing for final checkin
</commit_message>
<xml_diff>
--- a/testData/LoginDetails.xlsx
+++ b/testData/LoginDetails.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyWorkspace\CH\Sdem\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{755161F5-CDA1-411E-9493-9E25C9DAAC0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC41033E-18D0-4F8C-8BF8-814E397B15A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="19386" windowHeight="11466" activeTab="1" xr2:uid="{87D44E5E-FA58-43B3-A207-EC33F8C5A14B}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="19386" windowHeight="11466" xr2:uid="{87D44E5E-FA58-43B3-A207-EC33F8C5A14B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -75,13 +75,13 @@
     <t>postcode</t>
   </si>
   <si>
-    <t>Rahul</t>
-  </si>
-  <si>
-    <t>Ranjan</t>
-  </si>
-  <si>
     <t>CF117JA</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>User</t>
   </si>
 </sst>
 </file>
@@ -492,8 +492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19A20C3A-1312-45F7-930F-0D0FFFD0E31D}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -567,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B06B09C9-4D0C-4F9F-89B3-2D341B62C994}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -602,13 +602,13 @@
         <v>8</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>